<commit_message>
Corrected the values of Variance and Standard Deviation
There was an error on the excel when calculating the sum of squares that
was affecting the overall result, (forgot to substract the difference
with xbar) hence the SS, Variance and SD were not correct affecting the
final t-statistic value.
</commit_message>
<xml_diff>
--- a/Project 1 Test a Perceptual Phenomenon/P1 Data.xlsx
+++ b/Project 1 Test a Perceptual Phenomenon/P1 Data.xlsx
@@ -192,22 +192,10 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>(X</t>
+      <t>((X</t>
     </r>
     <r>
       <rPr>
@@ -253,7 +241,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>)</t>
+      <t>) - xbar)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
     </r>
   </si>
 </sst>
@@ -261,7 +261,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,6 +273,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -303,8 +310,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,12 +328,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -341,28 +361,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1103,18 +1142,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
@@ -1139,10 +1176,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1157,8 +1194,8 @@
         <v>-7.1989999999999981</v>
       </c>
       <c r="D3">
-        <f>C3*C3</f>
-        <v>51.82560099999997</v>
+        <f>(C3-(-7.96))^2</f>
+        <v>0.57912100000000288</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1173,8 +1210,8 @@
         <v>-1.9499999999999993</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D26" si="1">C4*C4</f>
-        <v>3.8024999999999971</v>
+        <f t="shared" ref="D4:D26" si="1">(C4-(-7.96))^2</f>
+        <v>36.120100000000008</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1190,7 +1227,7 @@
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>135.72249999999997</v>
+        <v>13.616099999999991</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1206,7 +1243,7 @@
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>49.801248999999977</v>
+        <v>0.81540900000000249</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1222,7 +1259,7 @@
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>66.161956000000004</v>
+        <v>3.0276000000000133E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1238,7 +1275,7 @@
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>74.649600000000007</v>
+        <v>0.46240000000000081</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1254,7 +1291,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>97.614399999999975</v>
+        <v>3.6863999999999963</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1270,7 +1307,7 @@
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>70.677648999999974</v>
+        <v>0.19980899999999846</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1286,7 +1323,7 @@
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>129.07232100000002</v>
+        <v>11.566801000000005</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1302,7 +1339,7 @@
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>139.287204</v>
+        <v>14.760963999999998</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1318,7 +1355,7 @@
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>4.8224160000000067</v>
+        <v>33.223695999999983</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1334,7 +1371,7 @@
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>11.195715999999988</v>
+        <v>21.288996000000015</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1350,7 +1387,7 @@
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>5.9389690000000055</v>
+        <v>30.503528999999986</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1366,7 +1403,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>11.566800999999998</v>
+        <v>20.784481000000003</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1382,7 +1419,7 @@
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>290.8730250000001</v>
+        <v>82.719025000000045</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1398,7 +1435,7 @@
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
-        <v>100.56078400000001</v>
+        <v>4.2766240000000018</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1414,7 +1451,7 @@
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>44.142735999999978</v>
+        <v>1.7318560000000043</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1430,7 +1467,7 @@
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>95.844099999999983</v>
+        <v>3.3488999999999969</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1446,7 +1483,7 @@
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
-        <v>36.978561000000013</v>
+        <v>3.5306409999999948</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1462,7 +1499,7 @@
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
-        <v>480.44256099999984</v>
+        <v>194.85368099999988</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1478,7 +1515,7 @@
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>119.90249999999995</v>
+        <v>8.9400999999999851</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1494,7 +1531,7 @@
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>13.890529000000003</v>
+        <v>17.918288999999998</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1510,7 +1547,7 @@
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
-        <v>5.5131039999999949</v>
+        <v>31.494544000000012</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1526,29 +1563,31 @@
       </c>
       <c r="D26">
         <f t="shared" si="1"/>
-        <v>26.553408999999988</v>
-      </c>
-      <c r="E26" s="1" t="s">
+        <v>7.8792490000000068</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="E27" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="C27" s="1" t="s">
+    <row r="28" spans="1:7">
+      <c r="C28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <f>SUM(D3:D26)</f>
-        <v>2066.8401909999993</v>
-      </c>
-      <c r="E27">
-        <f>D27/23</f>
-        <v>89.862616999999972</v>
-      </c>
-      <c r="F27">
-        <f>SQRT(E27)</f>
-        <v>9.4795894953315347</v>
-      </c>
-      <c r="G27" s="6" t="s">
+        <v>544.33099099999993</v>
+      </c>
+      <c r="E28" s="11">
+        <f>D28/23</f>
+        <v>23.666564826086955</v>
+      </c>
+      <c r="F28">
+        <f>SQRT(E28)</f>
+        <v>4.8648293727619016</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>